<commit_message>
make grade excel file look similar to grade pdf file
</commit_message>
<xml_diff>
--- a/public/templates/grade.xlsx
+++ b/public/templates/grade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\SideProjects\report-projects\att-manager\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E66145-F49B-4949-9491-0CB4E5DDE72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEC59C6-0172-42D6-BE0F-D012FDEB5E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21936" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21948" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>דוח ציונים ${group.klass.name} ${group.teacher.name} ${group.lesson.name}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>שם/ תאריך</t>
   </si>
@@ -48,6 +37,12 @@
   </si>
   <si>
     <t>${table:students.tz}</t>
+  </si>
+  <si>
+    <t>${title}</t>
+  </si>
+  <si>
+    <t>${headers}</t>
   </si>
 </sst>
 </file>
@@ -94,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -132,37 +127,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +459,7 @@
   <dimension ref="A1:E320"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A320"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -490,971 +469,977 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="4"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="4"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="4"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="4"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="4"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="4"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="A25" s="4"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="4"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+      <c r="A27" s="4"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="4"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="4"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="4"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+      <c r="A31" s="4"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+      <c r="A33" s="4"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="A34" s="4"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="A35" s="4"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="A36" s="4"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="4"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+      <c r="A38" s="4"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
+      <c r="A39" s="4"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="A40" s="4"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="A41" s="4"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
+      <c r="A42" s="4"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+      <c r="A43" s="4"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="A44" s="4"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="A45" s="4"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="A46" s="4"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="A47" s="4"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="A50" s="4"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="A51" s="4"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
+      <c r="A52" s="4"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
+      <c r="A53" s="4"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
+      <c r="A54" s="4"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
+      <c r="A55" s="4"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
+      <c r="A56" s="4"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
+      <c r="A57" s="4"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
+      <c r="A58" s="4"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
+      <c r="A59" s="4"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
+      <c r="A60" s="4"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
+      <c r="A61" s="4"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
+      <c r="A62" s="4"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
+      <c r="A63" s="4"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
+      <c r="A64" s="4"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
+      <c r="A65" s="4"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
+      <c r="A66" s="4"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
+      <c r="A67" s="4"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
+      <c r="A68" s="4"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
+      <c r="A69" s="4"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
+      <c r="A70" s="4"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
+      <c r="A71" s="4"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
+      <c r="A72" s="4"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
+      <c r="A73" s="4"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
+      <c r="A74" s="4"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
+      <c r="A75" s="4"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
+      <c r="A76" s="4"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
+      <c r="A77" s="4"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
+      <c r="A78" s="4"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
+      <c r="A79" s="4"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
+      <c r="A80" s="4"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="6"/>
+      <c r="A81" s="4"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="6"/>
+      <c r="A82" s="4"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="6"/>
+      <c r="A83" s="4"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
+      <c r="A84" s="4"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="6"/>
+      <c r="A85" s="4"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="6"/>
+      <c r="A86" s="4"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="6"/>
+      <c r="A87" s="4"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="6"/>
+      <c r="A88" s="4"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="6"/>
+      <c r="A89" s="4"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="6"/>
+      <c r="A90" s="4"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="6"/>
+      <c r="A91" s="4"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="6"/>
+      <c r="A92" s="4"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
+      <c r="A93" s="4"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="6"/>
+      <c r="A94" s="4"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="6"/>
+      <c r="A95" s="4"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="6"/>
+      <c r="A96" s="4"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="6"/>
+      <c r="A97" s="4"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="6"/>
+      <c r="A98" s="4"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="6"/>
+      <c r="A99" s="4"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="6"/>
+      <c r="A100" s="4"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="6"/>
+      <c r="A101" s="4"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="6"/>
+      <c r="A102" s="4"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="6"/>
+      <c r="A103" s="4"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="6"/>
+      <c r="A104" s="4"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="6"/>
+      <c r="A105" s="4"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
+      <c r="A106" s="4"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="6"/>
+      <c r="A107" s="4"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="6"/>
+      <c r="A108" s="4"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="6"/>
+      <c r="A109" s="4"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="6"/>
+      <c r="A110" s="4"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="6"/>
+      <c r="A111" s="4"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="6"/>
+      <c r="A112" s="4"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="6"/>
+      <c r="A113" s="4"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="6"/>
+      <c r="A114" s="4"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="6"/>
+      <c r="A115" s="4"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="6"/>
+      <c r="A116" s="4"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="6"/>
+      <c r="A117" s="4"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="6"/>
+      <c r="A118" s="4"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="6"/>
+      <c r="A119" s="4"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="6"/>
+      <c r="A120" s="4"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="6"/>
+      <c r="A121" s="4"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="6"/>
+      <c r="A122" s="4"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="6"/>
+      <c r="A123" s="4"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="6"/>
+      <c r="A124" s="4"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="6"/>
+      <c r="A125" s="4"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="6"/>
+      <c r="A126" s="4"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="6"/>
+      <c r="A127" s="4"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="6"/>
+      <c r="A128" s="4"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="6"/>
+      <c r="A129" s="4"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="6"/>
+      <c r="A130" s="4"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="6"/>
+      <c r="A131" s="4"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="6"/>
+      <c r="A132" s="4"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="6"/>
+      <c r="A133" s="4"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="6"/>
+      <c r="A134" s="4"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="6"/>
+      <c r="A135" s="4"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="6"/>
+      <c r="A136" s="4"/>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="6"/>
+      <c r="A137" s="4"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="6"/>
+      <c r="A138" s="4"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="6"/>
+      <c r="A139" s="4"/>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="6"/>
+      <c r="A140" s="4"/>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="6"/>
+      <c r="A141" s="4"/>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="6"/>
+      <c r="A142" s="4"/>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="6"/>
+      <c r="A143" s="4"/>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="6"/>
+      <c r="A144" s="4"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="6"/>
+      <c r="A145" s="4"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="6"/>
+      <c r="A146" s="4"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="6"/>
+      <c r="A147" s="4"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="6"/>
+      <c r="A148" s="4"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="6"/>
+      <c r="A149" s="4"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="6"/>
+      <c r="A150" s="4"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="6"/>
+      <c r="A151" s="4"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="6"/>
+      <c r="A152" s="4"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="6"/>
+      <c r="A153" s="4"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="6"/>
+      <c r="A154" s="4"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="6"/>
+      <c r="A155" s="4"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="6"/>
+      <c r="A156" s="4"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="6"/>
+      <c r="A157" s="4"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="6"/>
+      <c r="A158" s="4"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="6"/>
+      <c r="A159" s="4"/>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="6"/>
+      <c r="A160" s="4"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="6"/>
+      <c r="A161" s="4"/>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="6"/>
+      <c r="A162" s="4"/>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="6"/>
+      <c r="A163" s="4"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="6"/>
+      <c r="A164" s="4"/>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="6"/>
+      <c r="A165" s="4"/>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="6"/>
+      <c r="A166" s="4"/>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="6"/>
+      <c r="A167" s="4"/>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="6"/>
+      <c r="A168" s="4"/>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="6"/>
+      <c r="A169" s="4"/>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="6"/>
+      <c r="A170" s="4"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="6"/>
+      <c r="A171" s="4"/>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="6"/>
+      <c r="A172" s="4"/>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="6"/>
+      <c r="A173" s="4"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="6"/>
+      <c r="A174" s="4"/>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="6"/>
+      <c r="A175" s="4"/>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="6"/>
+      <c r="A176" s="4"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="6"/>
+      <c r="A177" s="4"/>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="6"/>
+      <c r="A178" s="4"/>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="6"/>
+      <c r="A179" s="4"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="6"/>
+      <c r="A180" s="4"/>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="6"/>
+      <c r="A181" s="4"/>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="6"/>
+      <c r="A182" s="4"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="6"/>
+      <c r="A183" s="4"/>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="6"/>
+      <c r="A184" s="4"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="6"/>
+      <c r="A185" s="4"/>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="6"/>
+      <c r="A186" s="4"/>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="6"/>
+      <c r="A187" s="4"/>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="6"/>
+      <c r="A188" s="4"/>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="6"/>
+      <c r="A189" s="4"/>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="6"/>
+      <c r="A190" s="4"/>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="6"/>
+      <c r="A191" s="4"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="6"/>
+      <c r="A192" s="4"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="6"/>
+      <c r="A193" s="4"/>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="6"/>
+      <c r="A194" s="4"/>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="6"/>
+      <c r="A195" s="4"/>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="6"/>
+      <c r="A196" s="4"/>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="6"/>
+      <c r="A197" s="4"/>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="6"/>
+      <c r="A198" s="4"/>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="6"/>
+      <c r="A199" s="4"/>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="6"/>
+      <c r="A200" s="4"/>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="6"/>
+      <c r="A201" s="4"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="6"/>
+      <c r="A202" s="4"/>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="6"/>
+      <c r="A203" s="4"/>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="6"/>
+      <c r="A204" s="4"/>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="6"/>
+      <c r="A205" s="4"/>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="6"/>
+      <c r="A206" s="4"/>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="6"/>
+      <c r="A207" s="4"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="6"/>
+      <c r="A208" s="4"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="6"/>
+      <c r="A209" s="4"/>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="6"/>
+      <c r="A210" s="4"/>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="6"/>
+      <c r="A211" s="4"/>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="6"/>
+      <c r="A212" s="4"/>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="6"/>
+      <c r="A213" s="4"/>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="6"/>
+      <c r="A214" s="4"/>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" s="6"/>
+      <c r="A215" s="4"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="6"/>
+      <c r="A216" s="4"/>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="6"/>
+      <c r="A217" s="4"/>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="6"/>
+      <c r="A218" s="4"/>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="6"/>
+      <c r="A219" s="4"/>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="6"/>
+      <c r="A220" s="4"/>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" s="6"/>
+      <c r="A221" s="4"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="6"/>
+      <c r="A222" s="4"/>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="6"/>
+      <c r="A223" s="4"/>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="6"/>
+      <c r="A224" s="4"/>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="6"/>
+      <c r="A225" s="4"/>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="6"/>
+      <c r="A226" s="4"/>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="6"/>
+      <c r="A227" s="4"/>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" s="6"/>
+      <c r="A228" s="4"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="6"/>
+      <c r="A229" s="4"/>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="6"/>
+      <c r="A230" s="4"/>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" s="6"/>
+      <c r="A231" s="4"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="6"/>
+      <c r="A232" s="4"/>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="6"/>
+      <c r="A233" s="4"/>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="6"/>
+      <c r="A234" s="4"/>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="6"/>
+      <c r="A235" s="4"/>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="6"/>
+      <c r="A236" s="4"/>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" s="6"/>
+      <c r="A237" s="4"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="6"/>
+      <c r="A238" s="4"/>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="6"/>
+      <c r="A239" s="4"/>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" s="6"/>
+      <c r="A240" s="4"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="6"/>
+      <c r="A241" s="4"/>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" s="6"/>
+      <c r="A242" s="4"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="6"/>
+      <c r="A243" s="4"/>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="6"/>
+      <c r="A244" s="4"/>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="6"/>
+      <c r="A245" s="4"/>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="6"/>
+      <c r="A246" s="4"/>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="6"/>
+      <c r="A247" s="4"/>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="6"/>
+      <c r="A248" s="4"/>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" s="6"/>
+      <c r="A249" s="4"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="6"/>
+      <c r="A250" s="4"/>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="6"/>
+      <c r="A251" s="4"/>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="6"/>
+      <c r="A252" s="4"/>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="6"/>
+      <c r="A253" s="4"/>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="6"/>
+      <c r="A254" s="4"/>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="6"/>
+      <c r="A255" s="4"/>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="6"/>
+      <c r="A256" s="4"/>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="6"/>
+      <c r="A257" s="4"/>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="6"/>
+      <c r="A258" s="4"/>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" s="6"/>
+      <c r="A259" s="4"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="6"/>
+      <c r="A260" s="4"/>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="6"/>
+      <c r="A261" s="4"/>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="6"/>
+      <c r="A262" s="4"/>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="6"/>
+      <c r="A263" s="4"/>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="6"/>
+      <c r="A264" s="4"/>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" s="6"/>
+      <c r="A265" s="4"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="6"/>
+      <c r="A266" s="4"/>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="6"/>
+      <c r="A267" s="4"/>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="6"/>
+      <c r="A268" s="4"/>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="6"/>
+      <c r="A269" s="4"/>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="6"/>
+      <c r="A270" s="4"/>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="6"/>
+      <c r="A271" s="4"/>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="6"/>
+      <c r="A272" s="4"/>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" s="6"/>
+      <c r="A273" s="4"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="6"/>
+      <c r="A274" s="4"/>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="6"/>
+      <c r="A275" s="4"/>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="6"/>
+      <c r="A276" s="4"/>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="6"/>
+      <c r="A277" s="4"/>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="6"/>
+      <c r="A278" s="4"/>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" s="6"/>
+      <c r="A279" s="4"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="6"/>
+      <c r="A280" s="4"/>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="6"/>
+      <c r="A281" s="4"/>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="6"/>
+      <c r="A282" s="4"/>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="6"/>
+      <c r="A283" s="4"/>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="6"/>
+      <c r="A284" s="4"/>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="6"/>
+      <c r="A285" s="4"/>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" s="6"/>
+      <c r="A286" s="4"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="6"/>
+      <c r="A287" s="4"/>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="6"/>
+      <c r="A288" s="4"/>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" s="6"/>
+      <c r="A289" s="4"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="6"/>
+      <c r="A290" s="4"/>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="6"/>
+      <c r="A291" s="4"/>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="6"/>
+      <c r="A292" s="4"/>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="6"/>
+      <c r="A293" s="4"/>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="6"/>
+      <c r="A294" s="4"/>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" s="6"/>
+      <c r="A295" s="4"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="6"/>
+      <c r="A296" s="4"/>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="6"/>
+      <c r="A297" s="4"/>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" s="6"/>
+      <c r="A298" s="4"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="6"/>
+      <c r="A299" s="4"/>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" s="6"/>
+      <c r="A300" s="4"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="6"/>
+      <c r="A301" s="4"/>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="6"/>
+      <c r="A302" s="4"/>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="6"/>
+      <c r="A303" s="4"/>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="6"/>
+      <c r="A304" s="4"/>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="6"/>
+      <c r="A305" s="4"/>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="6"/>
+      <c r="A306" s="4"/>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="6"/>
+      <c r="A307" s="4"/>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" s="6"/>
+      <c r="A308" s="4"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="6"/>
+      <c r="A309" s="4"/>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="6"/>
+      <c r="A310" s="4"/>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="6"/>
+      <c r="A311" s="4"/>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="6"/>
+      <c r="A312" s="4"/>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="6"/>
+      <c r="A313" s="4"/>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="6"/>
+      <c r="A314" s="4"/>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="6"/>
+      <c r="A315" s="4"/>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="6"/>
+      <c r="A316" s="4"/>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="6"/>
+      <c r="A317" s="4"/>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" s="6"/>
+      <c r="A318" s="4"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="6"/>
+      <c r="A319" s="4"/>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="6"/>
+      <c r="A320" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update grade excel template
</commit_message>
<xml_diff>
--- a/public/templates/grade.xlsx
+++ b/public/templates/grade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\SideProjects\report-projects\att-manager\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964AE30B-6561-4615-8FE2-28684E59D4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6624199-8285-4495-88ED-F3560CE33BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21948" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
   </bookViews>
@@ -149,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -171,6 +171,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -199,8 +202,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>60613</xdr:rowOff>
     </xdr:to>
@@ -538,14 +541,14 @@
   <dimension ref="A1:E322"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="13.69921875" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="5.296875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -586,7 +589,7 @@
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="12" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>